<commit_message>
Add zero counts to test cases for prediction
</commit_message>
<xml_diff>
--- a/Data/Processed/hd_hand_counted.xlsx
+++ b/Data/Processed/hd_hand_counted.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/h2lifespan/Data/Processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kingeg/Documents/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="460" windowWidth="16580" windowHeight="17300" tabRatio="500"/>
+    <workbookView xWindow="22140" yWindow="1540" windowWidth="19420" windowHeight="26900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="357">
   <si>
     <t>sampleid</t>
   </si>
@@ -1065,6 +1065,39 @@
   </si>
   <si>
     <t>camera_id</t>
+  </si>
+  <si>
+    <t>IMG_5548.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5273.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5323.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5432.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5154.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5460.JPG</t>
+  </si>
+  <si>
+    <t>IMG_4357.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5151.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5587.JPG</t>
+  </si>
+  <si>
+    <t>IMG_5488.JPG</t>
+  </si>
+  <si>
+    <t>EK</t>
   </si>
 </sst>
 </file>
@@ -1417,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J184"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F193" sqref="F193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5412,6 +5445,146 @@
         <v>35</v>
       </c>
     </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>346</v>
+      </c>
+      <c r="G185" s="1">
+        <v>0</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>347</v>
+      </c>
+      <c r="G186" s="1">
+        <v>0</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>348</v>
+      </c>
+      <c r="G187" s="1">
+        <v>0</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>349</v>
+      </c>
+      <c r="G188" s="1">
+        <v>0</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>350</v>
+      </c>
+      <c r="G189" s="1">
+        <v>0</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>351</v>
+      </c>
+      <c r="G190" s="1">
+        <v>0</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>352</v>
+      </c>
+      <c r="G191" s="1">
+        <v>0</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>353</v>
+      </c>
+      <c r="G192" s="1">
+        <v>0</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>354</v>
+      </c>
+      <c r="G193" s="1">
+        <v>0</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>355</v>
+      </c>
+      <c r="G194" s="1">
+        <v>0</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J162">
     <sortCondition ref="A2:A162"/>

</xml_diff>

<commit_message>
prediction files updated and new files added
</commit_message>
<xml_diff>
--- a/Data/Processed/hd_hand_counted.xlsx
+++ b/Data/Processed/hd_hand_counted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="620" windowWidth="19420" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="9380" yWindow="460" windowWidth="19420" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="409">
   <si>
     <t>sampleid</t>
   </si>
@@ -1098,13 +1098,169 @@
   </si>
   <si>
     <t>EK</t>
+  </si>
+  <si>
+    <t>IMG_2043.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2049.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2124.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2137.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2139.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2142.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2178.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2239.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2372.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2373.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2375.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2469.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2691.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2751.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2756.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2822.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2857.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2858.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2859.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2860.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2898.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2899.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2916.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2921.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2933.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2934.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2935.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2938.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3035.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3056.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3085.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3102.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3206.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3234.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3316.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3317.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3318.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3319.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3320.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3349.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3442.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3565.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3601.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3663.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3840.JPG</t>
+  </si>
+  <si>
+    <t>too dark</t>
+  </si>
+  <si>
+    <t>dense&amp;clumped</t>
+  </si>
+  <si>
+    <t>highlight on side</t>
+  </si>
+  <si>
+    <t>highlight</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>dark &amp; grid</t>
+  </si>
+  <si>
+    <t>no eggs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1142,6 +1298,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1163,7 +1326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1173,6 +1336,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1450,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I244" sqref="I244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3260,7 +3424,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>195</v>
       </c>
@@ -3283,7 +3447,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>194</v>
       </c>
@@ -3306,7 +3470,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>193</v>
       </c>
@@ -3329,7 +3493,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>192</v>
       </c>
@@ -3352,7 +3516,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
@@ -3375,7 +3539,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>190</v>
       </c>
@@ -3398,7 +3562,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>189</v>
       </c>
@@ -3421,7 +3585,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>188</v>
       </c>
@@ -3444,7 +3608,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>187</v>
       </c>
@@ -3467,7 +3631,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>204</v>
       </c>
@@ -3490,7 +3654,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>203</v>
       </c>
@@ -3513,7 +3677,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>202</v>
       </c>
@@ -3536,7 +3700,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>201</v>
       </c>
@@ -3559,7 +3723,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>200</v>
       </c>
@@ -3581,8 +3745,11 @@
       <c r="H94" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>199</v>
       </c>
@@ -3605,7 +3772,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>198</v>
       </c>
@@ -5557,7 +5724,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>354</v>
       </c>
@@ -5571,7 +5738,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>355</v>
       </c>
@@ -5583,6 +5750,755 @@
       </c>
       <c r="I194" s="1" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A195" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="G195" s="9">
+        <v>780</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J195" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A196" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G196" s="9">
+        <v>1354</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J196"/>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A197" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="G197" s="9">
+        <v>745</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J197" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A198" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="G198" s="9">
+        <v>808</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I198" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J198"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A199" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G199" s="9">
+        <v>1062</v>
+      </c>
+      <c r="H199" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I199" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J199"/>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A200" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="G200" s="9">
+        <v>1057</v>
+      </c>
+      <c r="H200" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I200" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J200"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A201" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G201" s="9">
+        <v>2073</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I201" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J201" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A202" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="G202" s="9">
+        <v>401</v>
+      </c>
+      <c r="H202" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I202" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J202" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A203" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G203" s="9">
+        <v>1578</v>
+      </c>
+      <c r="H203" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I203" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J203" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A204" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G204" s="9">
+        <v>819</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I204" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J204" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A205" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="G205" s="9">
+        <v>425</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I205" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J205" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A206" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G206" s="9">
+        <v>715</v>
+      </c>
+      <c r="H206" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I206" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J206" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A207" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G207" s="9">
+        <v>120</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I207" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J207" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A208" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="G208" s="9">
+        <v>830</v>
+      </c>
+      <c r="H208" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I208" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J208" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A209" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="G209" s="9">
+        <v>1065</v>
+      </c>
+      <c r="H209" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I209" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J209" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A210" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G210" s="9">
+        <v>157</v>
+      </c>
+      <c r="H210" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I210" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J210" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A211" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G211" s="9">
+        <v>853</v>
+      </c>
+      <c r="H211" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I211" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J211" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A212" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="G212" s="9">
+        <v>526</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I212" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J212" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A213" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G213" s="9">
+        <v>195</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I213" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J213" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A214" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G214" s="9">
+        <v>368</v>
+      </c>
+      <c r="H214" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I214" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J214" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A215" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="G215" s="9">
+        <v>338</v>
+      </c>
+      <c r="H215" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I215" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J215" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A216" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="G216" s="9">
+        <v>85</v>
+      </c>
+      <c r="H216" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I216" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J216" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A217" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="G217" s="9">
+        <v>647</v>
+      </c>
+      <c r="H217" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I217" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J217" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A218" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="G218" s="9">
+        <v>208</v>
+      </c>
+      <c r="H218" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I218" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J218"/>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A219" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="G219" s="9">
+        <v>841</v>
+      </c>
+      <c r="H219" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I219" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J219" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A220" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="G220" s="9">
+        <v>770</v>
+      </c>
+      <c r="H220" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I220" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J220" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A221" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="G221" s="9">
+        <v>747</v>
+      </c>
+      <c r="H221" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I221" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J221" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A222" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="G222" s="9">
+        <v>326</v>
+      </c>
+      <c r="H222" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I222" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J222" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A223" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="G223" s="9">
+        <v>938</v>
+      </c>
+      <c r="H223" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I223" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J223"/>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A224" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="G224" s="9">
+        <v>978</v>
+      </c>
+      <c r="H224" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I224" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J224"/>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A225" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="G225" s="9">
+        <v>985</v>
+      </c>
+      <c r="H225" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I225" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J225" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A226" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="G226" s="9">
+        <v>631</v>
+      </c>
+      <c r="H226" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I226" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J226" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A227" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="G227" s="9">
+        <v>572</v>
+      </c>
+      <c r="H227" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I227" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J227" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A228" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="G228" s="9">
+        <v>409</v>
+      </c>
+      <c r="H228" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I228" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J228" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A229" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="G229" s="9">
+        <v>613</v>
+      </c>
+      <c r="H229" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I229" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J229" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A230" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="G230" s="9">
+        <v>566</v>
+      </c>
+      <c r="H230" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I230" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J230" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A231" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="G231" s="9">
+        <v>432</v>
+      </c>
+      <c r="H231" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I231" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J231" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A232" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="G232" s="9">
+        <v>427</v>
+      </c>
+      <c r="H232" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I232" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J232" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A233" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="G233" s="9">
+        <v>344</v>
+      </c>
+      <c r="H233" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I233" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J233" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A234" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="G234" s="9">
+        <v>459</v>
+      </c>
+      <c r="H234" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I234" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J234" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A235" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G235" s="9">
+        <v>1134</v>
+      </c>
+      <c r="H235" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I235" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J235"/>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A236" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="G236" s="9">
+        <v>324</v>
+      </c>
+      <c r="H236" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I236" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J236" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A237" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="G237" s="9">
+        <v>7</v>
+      </c>
+      <c r="H237" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I237" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J237" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A238" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="G238" s="9">
+        <v>66</v>
+      </c>
+      <c r="H238" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I238" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J238" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A239" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="G239" s="9">
+        <v>107</v>
+      </c>
+      <c r="H239" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I239" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J239" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>